<commit_message>
Keep fairness metric asymmetric to remove cancellation across buckets
</commit_message>
<xml_diff>
--- a/results/classification_simulations.xlsx
+++ b/results/classification_simulations.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arushi Jain\MIT Dropbox\Arushi Jain\FairAI\results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97F64B4-7E46-4E2B-B910-A9A5E8B4769D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -121,8 +127,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,15 +189,34 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -229,7 +254,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -263,6 +288,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -297,9 +323,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -472,14 +499,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,7 +534,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -525,13 +554,13 @@
         <v>1987</v>
       </c>
       <c r="G2">
-        <v>0.9759712916092375</v>
+        <v>0.97597129160923746</v>
       </c>
       <c r="H2">
-        <v>0.9908819500003527</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>0.99088195000035273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -551,13 +580,13 @@
         <v>2014</v>
       </c>
       <c r="G3">
-        <v>0.9584934697634336</v>
+        <v>0.95849346976343364</v>
       </c>
       <c r="H3">
-        <v>0.9917754719414292</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>0.99177547194142923</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -577,13 +606,13 @@
         <v>1999</v>
       </c>
       <c r="G4">
-        <v>0.9814292344953536</v>
+        <v>0.98142923449535358</v>
       </c>
       <c r="H4">
-        <v>0.9973411892843893</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>0.99734118928438931</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -603,13 +632,13 @@
         <v>1984</v>
       </c>
       <c r="G5">
-        <v>0.9972023266971465</v>
+        <v>0.99720232669714648</v>
       </c>
       <c r="H5">
-        <v>0.8726057499860828</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>0.87260574998608276</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -629,13 +658,13 @@
         <v>2007</v>
       </c>
       <c r="G6">
-        <v>0.9927938788196302</v>
+        <v>0.99279387881963022</v>
       </c>
       <c r="H6">
         <v>0.9344752146901365</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -655,13 +684,13 @@
         <v>2009</v>
       </c>
       <c r="G7">
-        <v>0.9954196894788453</v>
+        <v>0.99541968947884529</v>
       </c>
       <c r="H7">
-        <v>0.9372368081529902</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>0.93723680815299015</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -681,13 +710,13 @@
         <v>2028</v>
       </c>
       <c r="G8">
-        <v>0.8750535049231796</v>
+        <v>0.87505350492317957</v>
       </c>
       <c r="H8">
-        <v>0.9107716877628403</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>0.91077168776284034</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -707,13 +736,13 @@
         <v>1971</v>
       </c>
       <c r="G9">
-        <v>0.9384016682731295</v>
+        <v>0.93840166827312954</v>
       </c>
       <c r="H9">
-        <v>0.9552890601361609</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>0.95528906013616088</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -733,13 +762,13 @@
         <v>2001</v>
       </c>
       <c r="G10">
-        <v>0.926511852477902</v>
+        <v>0.92651185247790202</v>
       </c>
       <c r="H10">
-        <v>0.9484854761576039</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>0.94848547615760392</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -759,13 +788,13 @@
         <v>2042</v>
       </c>
       <c r="G11">
-        <v>0.9132852596339983</v>
+        <v>0.91328525963399831</v>
       </c>
       <c r="H11">
-        <v>0.7730436596575689</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>0.77304365965756894</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -785,13 +814,13 @@
         <v>1999</v>
       </c>
       <c r="G12">
-        <v>0.9547712252255038</v>
+        <v>0.95477122522550384</v>
       </c>
       <c r="H12">
-        <v>0.8764895688062649</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>0.87648956880626494</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -811,13 +840,13 @@
         <v>1959</v>
       </c>
       <c r="G13">
-        <v>0.9408596496138982</v>
+        <v>0.94085964961389823</v>
       </c>
       <c r="H13">
-        <v>0.8726268882132815</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>0.87262688821328149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -837,13 +866,13 @@
         <v>2400</v>
       </c>
       <c r="G14">
-        <v>0.9677937463505243</v>
+        <v>0.96779374635052429</v>
       </c>
       <c r="H14">
-        <v>0.9922898653279674</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>0.99228986532796737</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -863,13 +892,13 @@
         <v>2377</v>
       </c>
       <c r="G15">
-        <v>0.968936223387615</v>
+        <v>0.96893622338761498</v>
       </c>
       <c r="H15">
-        <v>0.9934406939050568</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>0.99344069390505685</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -889,13 +918,13 @@
         <v>1223</v>
       </c>
       <c r="G16">
-        <v>0.9726039597615826</v>
+        <v>0.97260395976158265</v>
       </c>
       <c r="H16">
-        <v>0.9898025871932032</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>0.98980258719320324</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -915,13 +944,13 @@
         <v>2383</v>
       </c>
       <c r="G17">
-        <v>0.9783512337259407</v>
+        <v>0.97835123372594068</v>
       </c>
       <c r="H17">
-        <v>0.9048045623491787</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>0.90480456234917872</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -941,13 +970,13 @@
         <v>2417</v>
       </c>
       <c r="G18">
-        <v>0.9857254672944694</v>
+        <v>0.98572546729446942</v>
       </c>
       <c r="H18">
-        <v>0.9456061913172831</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>0.94560619131728307</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -967,13 +996,13 @@
         <v>1200</v>
       </c>
       <c r="G19">
-        <v>0.9894052407275113</v>
+        <v>0.98940524072751135</v>
       </c>
       <c r="H19">
         <v>0.9378361317418823</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -993,13 +1022,13 @@
         <v>2309</v>
       </c>
       <c r="G20">
-        <v>0.8606516841374224</v>
+        <v>0.86065168413742243</v>
       </c>
       <c r="H20">
-        <v>0.9143285549747626</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>0.91432855497476262</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1019,13 +1048,13 @@
         <v>2499</v>
       </c>
       <c r="G21">
-        <v>0.896846962537614</v>
+        <v>0.89684696253761398</v>
       </c>
       <c r="H21">
-        <v>0.926984636391109</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>0.92698463639110895</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1045,13 +1074,13 @@
         <v>1192</v>
       </c>
       <c r="G22">
-        <v>0.9556327579315191</v>
+        <v>0.95563275793151914</v>
       </c>
       <c r="H22">
-        <v>0.9770217270800093</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>0.97702172708000934</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -1071,13 +1100,13 @@
         <v>2344</v>
       </c>
       <c r="G23">
-        <v>0.8729603261348641</v>
+        <v>0.87296032613486407</v>
       </c>
       <c r="H23">
-        <v>0.7725371074897677</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>0.77253710748976767</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -1097,13 +1126,13 @@
         <v>2479</v>
       </c>
       <c r="G24">
-        <v>0.9017797412040247</v>
+        <v>0.90177974120402471</v>
       </c>
       <c r="H24">
         <v>0.8327699113557111</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1123,13 +1152,13 @@
         <v>1177</v>
       </c>
       <c r="G25">
-        <v>0.9486751596995355</v>
+        <v>0.94867515969953553</v>
       </c>
       <c r="H25">
-        <v>0.8818588164301255</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>0.88185881643012554</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1149,13 +1178,13 @@
         <v>1987</v>
       </c>
       <c r="G26">
-        <v>0.9908268125239614</v>
+        <v>0.99082681252396143</v>
       </c>
       <c r="H26">
-        <v>0.9910737415241642</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>0.99107374152416416</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -1175,13 +1204,13 @@
         <v>2014</v>
       </c>
       <c r="G27">
-        <v>0.9823541320417736</v>
+        <v>0.98235413204177358</v>
       </c>
       <c r="H27">
-        <v>0.9944680671301483</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>0.99446806713014835</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -1204,10 +1233,10 @@
         <v>0.9808451740120272</v>
       </c>
       <c r="H28">
-        <v>0.9877123333837688</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>0.98771233338376885</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -1230,10 +1259,10 @@
         <v>0.9666830195688233</v>
       </c>
       <c r="H29">
-        <v>0.8400972713047526</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>0.84009727130475265</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1253,13 +1282,13 @@
         <v>2007</v>
       </c>
       <c r="G30">
-        <v>0.9739459373076387</v>
+        <v>0.97394593730763868</v>
       </c>
       <c r="H30">
-        <v>0.9293912316493433</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>0.92939123164934334</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -1279,13 +1308,13 @@
         <v>2009</v>
       </c>
       <c r="G31">
-        <v>0.9881930993620296</v>
+        <v>0.98819309936202959</v>
       </c>
       <c r="H31">
         <v>0.9052760891512609</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1305,13 +1334,13 @@
         <v>2028</v>
       </c>
       <c r="G32">
-        <v>0.8669186206715446</v>
+        <v>0.86691862067154457</v>
       </c>
       <c r="H32">
-        <v>0.8768365551637285</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>0.87683655516372849</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1331,13 +1360,13 @@
         <v>1971</v>
       </c>
       <c r="G33">
-        <v>0.9474378597692178</v>
+        <v>0.94743785976921779</v>
       </c>
       <c r="H33">
-        <v>0.928594975779399</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>0.92859497577939898</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -1357,13 +1386,13 @@
         <v>2001</v>
       </c>
       <c r="G34">
-        <v>0.9183207508099476</v>
+        <v>0.91832075080994757</v>
       </c>
       <c r="H34">
-        <v>0.9398613584632873</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>0.93986135846328733</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -1383,13 +1412,13 @@
         <v>2042</v>
       </c>
       <c r="G35">
-        <v>0.9153605083516773</v>
+        <v>0.91536050835167726</v>
       </c>
       <c r="H35">
-        <v>0.6976180373564311</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+        <v>0.69761803735643113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -1409,13 +1438,13 @@
         <v>1999</v>
       </c>
       <c r="G36">
-        <v>0.9519645056567684</v>
+        <v>0.95196450565676838</v>
       </c>
       <c r="H36">
-        <v>0.8258722059337786</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+        <v>0.82587220593377864</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -1435,13 +1464,18 @@
         <v>1959</v>
       </c>
       <c r="G37">
-        <v>0.9490270449402304</v>
+        <v>0.94902704494023038</v>
       </c>
       <c r="H37">
-        <v>0.8333908906492475</v>
+        <v>0.83339089064924754</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0.8</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor classification synthetic data generation
</commit_message>
<xml_diff>
--- a/results/classification_simulations.xlsx
+++ b/results/classification_simulations.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arushi Jain\MIT Dropbox\Arushi Jain\FairAI\results\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97F64B4-7E46-4E2B-B910-A9A5E8B4769D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -106,7 +100,7 @@
     <t>(0.34, 0.33, 0.33)</t>
   </si>
   <si>
-    <t>[0.34, 0.33, 0.33]</t>
+    <t>[0.33, 0.33, 0.33]</t>
   </si>
   <si>
     <t>[0.2, 0.5, 0.3]</t>
@@ -127,8 +121,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,34 +183,15 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -254,7 +229,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -288,7 +263,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -323,10 +297,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -499,16 +472,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,7 +505,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -551,16 +522,16 @@
         <v>30</v>
       </c>
       <c r="F2">
-        <v>1987</v>
+        <v>1983</v>
       </c>
       <c r="G2">
-        <v>0.97597129160923746</v>
+        <v>0.9730663837782545</v>
       </c>
       <c r="H2">
-        <v>0.99088195000035273</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9953757150787123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -580,13 +551,13 @@
         <v>2014</v>
       </c>
       <c r="G3">
-        <v>0.95849346976343364</v>
+        <v>0.9792545727230993</v>
       </c>
       <c r="H3">
-        <v>0.99177547194142923</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9908263448068602</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -603,16 +574,16 @@
         <v>30</v>
       </c>
       <c r="F4">
-        <v>1999</v>
+        <v>2003</v>
       </c>
       <c r="G4">
-        <v>0.98142923449535358</v>
+        <v>0.9821234791256194</v>
       </c>
       <c r="H4">
-        <v>0.99734118928438931</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9916921031082567</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -629,16 +600,16 @@
         <v>31</v>
       </c>
       <c r="F5">
-        <v>1984</v>
+        <v>2008</v>
       </c>
       <c r="G5">
-        <v>0.99720232669714648</v>
+        <v>0.9799819065811723</v>
       </c>
       <c r="H5">
-        <v>0.87260574998608276</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.8763972190758041</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -655,16 +626,16 @@
         <v>30</v>
       </c>
       <c r="F6">
-        <v>2007</v>
+        <v>1972</v>
       </c>
       <c r="G6">
-        <v>0.99279387881963022</v>
+        <v>0.9820925564120693</v>
       </c>
       <c r="H6">
-        <v>0.9344752146901365</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9315771213971266</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -681,16 +652,16 @@
         <v>30</v>
       </c>
       <c r="F7">
-        <v>2009</v>
+        <v>2020</v>
       </c>
       <c r="G7">
-        <v>0.99541968947884529</v>
+        <v>0.9957869989718151</v>
       </c>
       <c r="H7">
-        <v>0.93723680815299015</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9414718933330611</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -707,16 +678,16 @@
         <v>32</v>
       </c>
       <c r="F8">
-        <v>2028</v>
+        <v>1897</v>
       </c>
       <c r="G8">
-        <v>0.87505350492317957</v>
+        <v>0.8569894699374928</v>
       </c>
       <c r="H8">
-        <v>0.91077168776284034</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9061259020888963</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -733,16 +704,16 @@
         <v>30</v>
       </c>
       <c r="F9">
-        <v>1971</v>
+        <v>2101</v>
       </c>
       <c r="G9">
-        <v>0.93840166827312954</v>
+        <v>0.9337302346033731</v>
       </c>
       <c r="H9">
-        <v>0.95528906013616088</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9476833479013603</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -759,16 +730,16 @@
         <v>30</v>
       </c>
       <c r="F10">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="G10">
-        <v>0.92651185247790202</v>
+        <v>0.9260077671576913</v>
       </c>
       <c r="H10">
-        <v>0.94848547615760392</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9579843375632696</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -785,16 +756,16 @@
         <v>33</v>
       </c>
       <c r="F11">
-        <v>2042</v>
+        <v>1929</v>
       </c>
       <c r="G11">
-        <v>0.91328525963399831</v>
+        <v>0.8742088238668536</v>
       </c>
       <c r="H11">
-        <v>0.77304365965756894</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.774184365108198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -811,16 +782,16 @@
         <v>30</v>
       </c>
       <c r="F12">
-        <v>1999</v>
+        <v>2081</v>
       </c>
       <c r="G12">
-        <v>0.95477122522550384</v>
+        <v>0.9374814945662673</v>
       </c>
       <c r="H12">
-        <v>0.87648956880626494</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.882061809996029</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -837,16 +808,16 @@
         <v>30</v>
       </c>
       <c r="F13">
-        <v>1959</v>
+        <v>1990</v>
       </c>
       <c r="G13">
-        <v>0.94085964961389823</v>
+        <v>0.9383284644306384</v>
       </c>
       <c r="H13">
-        <v>0.87262688821328149</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.8805044287834728</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -866,13 +837,13 @@
         <v>2400</v>
       </c>
       <c r="G14">
-        <v>0.96779374635052429</v>
+        <v>0.9677937463505243</v>
       </c>
       <c r="H14">
-        <v>0.99228986532796737</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9922898653279674</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -892,13 +863,13 @@
         <v>2377</v>
       </c>
       <c r="G15">
-        <v>0.96893622338761498</v>
+        <v>0.968936223387615</v>
       </c>
       <c r="H15">
-        <v>0.99344069390505685</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9934406939050568</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -918,13 +889,13 @@
         <v>1223</v>
       </c>
       <c r="G16">
-        <v>0.97260395976158265</v>
+        <v>0.9726039597615826</v>
       </c>
       <c r="H16">
-        <v>0.98980258719320324</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9898025871932032</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -944,13 +915,13 @@
         <v>2383</v>
       </c>
       <c r="G17">
-        <v>0.97835123372594068</v>
+        <v>0.9783512337259407</v>
       </c>
       <c r="H17">
-        <v>0.90480456234917872</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9048045623491787</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -970,13 +941,13 @@
         <v>2417</v>
       </c>
       <c r="G18">
-        <v>0.98572546729446942</v>
+        <v>0.9857254672944694</v>
       </c>
       <c r="H18">
-        <v>0.94560619131728307</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9456061913172831</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -996,13 +967,13 @@
         <v>1200</v>
       </c>
       <c r="G19">
-        <v>0.98940524072751135</v>
+        <v>0.9894052407275113</v>
       </c>
       <c r="H19">
         <v>0.9378361317418823</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1022,13 +993,13 @@
         <v>2309</v>
       </c>
       <c r="G20">
-        <v>0.86065168413742243</v>
+        <v>0.8606516841374224</v>
       </c>
       <c r="H20">
-        <v>0.91432855497476262</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9143285549747626</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1048,13 +1019,13 @@
         <v>2499</v>
       </c>
       <c r="G21">
-        <v>0.89684696253761398</v>
+        <v>0.896846962537614</v>
       </c>
       <c r="H21">
-        <v>0.92698463639110895</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.926984636391109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1074,13 +1045,13 @@
         <v>1192</v>
       </c>
       <c r="G22">
-        <v>0.95563275793151914</v>
+        <v>0.9556327579315191</v>
       </c>
       <c r="H22">
-        <v>0.97702172708000934</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9770217270800093</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -1100,13 +1071,13 @@
         <v>2344</v>
       </c>
       <c r="G23">
-        <v>0.87296032613486407</v>
+        <v>0.8729603261348641</v>
       </c>
       <c r="H23">
-        <v>0.77253710748976767</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.7725371074897677</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -1126,13 +1097,13 @@
         <v>2479</v>
       </c>
       <c r="G24">
-        <v>0.90177974120402471</v>
+        <v>0.9017797412040247</v>
       </c>
       <c r="H24">
         <v>0.8327699113557111</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1152,13 +1123,13 @@
         <v>1177</v>
       </c>
       <c r="G25">
-        <v>0.94867515969953553</v>
+        <v>0.9486751596995355</v>
       </c>
       <c r="H25">
-        <v>0.88185881643012554</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.8818588164301255</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1175,16 +1146,16 @@
         <v>30</v>
       </c>
       <c r="F26">
-        <v>1987</v>
+        <v>1983</v>
       </c>
       <c r="G26">
-        <v>0.99082681252396143</v>
+        <v>0.9822400994231908</v>
       </c>
       <c r="H26">
-        <v>0.99107374152416416</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9873068028819293</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -1204,13 +1175,13 @@
         <v>2014</v>
       </c>
       <c r="G27">
-        <v>0.98235413204177358</v>
+        <v>0.9875209121486256</v>
       </c>
       <c r="H27">
-        <v>0.99446806713014835</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9848426074188429</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -1227,16 +1198,16 @@
         <v>30</v>
       </c>
       <c r="F28">
-        <v>1999</v>
+        <v>2003</v>
       </c>
       <c r="G28">
-        <v>0.9808451740120272</v>
+        <v>0.9708017405676321</v>
       </c>
       <c r="H28">
-        <v>0.98771233338376885</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9893454395628996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -1253,16 +1224,16 @@
         <v>31</v>
       </c>
       <c r="F29">
-        <v>1984</v>
+        <v>2008</v>
       </c>
       <c r="G29">
-        <v>0.9666830195688233</v>
+        <v>0.9927928563867169</v>
       </c>
       <c r="H29">
-        <v>0.84009727130475265</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.8314686377483625</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1279,16 +1250,16 @@
         <v>30</v>
       </c>
       <c r="F30">
-        <v>2007</v>
+        <v>1972</v>
       </c>
       <c r="G30">
-        <v>0.97394593730763868</v>
+        <v>0.9806781541503131</v>
       </c>
       <c r="H30">
-        <v>0.92939123164934334</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9163805059369896</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -1305,16 +1276,16 @@
         <v>30</v>
       </c>
       <c r="F31">
-        <v>2009</v>
+        <v>2020</v>
       </c>
       <c r="G31">
-        <v>0.98819309936202959</v>
+        <v>0.9871933421244188</v>
       </c>
       <c r="H31">
-        <v>0.9052760891512609</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9109364091862266</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1331,16 +1302,16 @@
         <v>32</v>
       </c>
       <c r="F32">
-        <v>2028</v>
+        <v>1897</v>
       </c>
       <c r="G32">
-        <v>0.86691862067154457</v>
+        <v>0.8733483936198283</v>
       </c>
       <c r="H32">
-        <v>0.87683655516372849</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.893018296712767</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1357,16 +1328,16 @@
         <v>30</v>
       </c>
       <c r="F33">
-        <v>1971</v>
+        <v>2101</v>
       </c>
       <c r="G33">
-        <v>0.94743785976921779</v>
+        <v>0.9520549035942528</v>
       </c>
       <c r="H33">
-        <v>0.92859497577939898</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9398931018317949</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -1383,16 +1354,16 @@
         <v>30</v>
       </c>
       <c r="F34">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="G34">
-        <v>0.91832075080994757</v>
+        <v>0.9226737494192788</v>
       </c>
       <c r="H34">
-        <v>0.93986135846328733</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9532209597940299</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -1409,16 +1380,16 @@
         <v>33</v>
       </c>
       <c r="F35">
-        <v>2042</v>
+        <v>1929</v>
       </c>
       <c r="G35">
-        <v>0.91536050835167726</v>
+        <v>0.876566763544507</v>
       </c>
       <c r="H35">
-        <v>0.69761803735643113</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.6864097780382082</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -1435,16 +1406,16 @@
         <v>30</v>
       </c>
       <c r="F36">
-        <v>1999</v>
+        <v>2081</v>
       </c>
       <c r="G36">
-        <v>0.95196450565676838</v>
+        <v>0.9519017535880143</v>
       </c>
       <c r="H36">
-        <v>0.82587220593377864</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.8277898707885657</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -1461,21 +1432,16 @@
         <v>30</v>
       </c>
       <c r="F37">
-        <v>1959</v>
+        <v>1990</v>
       </c>
       <c r="G37">
-        <v>0.94902704494023038</v>
+        <v>0.925837185109776</v>
       </c>
       <c r="H37">
-        <v>0.83339089064924754</v>
+        <v>0.8396855433622178</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
-      <formula>0.8</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add global direction for interpetability
</commit_message>
<xml_diff>
--- a/results/classification_simulations.xlsx
+++ b/results/classification_simulations.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arushi Jain\MIT Dropbox\Arushi Jain\FairAI\results\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B56144F-4379-4364-BA32-D46DB7172F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="37">
   <si>
     <t>simulation_type</t>
   </si>
@@ -46,6 +40,9 @@
     <t>FairAI_pred</t>
   </si>
   <si>
+    <t>global_bias_direction</t>
+  </si>
+  <si>
     <t>high_bias_single_cat_equal_distribution_classification</t>
   </si>
   <si>
@@ -122,13 +119,19 @@
   </si>
   <si>
     <t>[0.5, 3, 1.5]</t>
+  </si>
+  <si>
+    <t>no bias</t>
+  </si>
+  <si>
+    <t>mixed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,34 +192,15 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -254,7 +238,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -288,7 +272,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -323,10 +306,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -499,16 +481,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,22 +513,25 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F2">
         <v>1983</v>
@@ -557,778 +540,868 @@
         <v>0.9730663837782545</v>
       </c>
       <c r="H2">
-        <v>0.99537571507871225</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9953757150787123</v>
+      </c>
+      <c r="I2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F3">
         <v>2014</v>
       </c>
       <c r="G3">
-        <v>0.97925457272309935</v>
+        <v>0.9792545727230993</v>
       </c>
       <c r="H3">
-        <v>0.99082634480686016</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9908263448068602</v>
+      </c>
+      <c r="I3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F4">
         <v>2003</v>
       </c>
       <c r="G4">
-        <v>0.98212347912561937</v>
+        <v>0.9821234791256194</v>
       </c>
       <c r="H4">
-        <v>0.99169210310825673</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9916921031082567</v>
+      </c>
+      <c r="I4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F5">
         <v>2008</v>
       </c>
       <c r="G5">
-        <v>0.97998190658117235</v>
+        <v>0.9799819065811723</v>
       </c>
       <c r="H5">
-        <v>0.87639721907580415</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.8763972190758041</v>
+      </c>
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F6">
         <v>1972</v>
       </c>
       <c r="G6">
-        <v>0.98209255641206927</v>
+        <v>0.9820925564120693</v>
       </c>
       <c r="H6">
-        <v>0.93157712139712656</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9315771213971266</v>
+      </c>
+      <c r="I6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F7">
         <v>2020</v>
       </c>
       <c r="G7">
-        <v>0.99578699897181511</v>
+        <v>0.9957869989718151</v>
       </c>
       <c r="H7">
-        <v>0.94147189333306114</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9414718933330611</v>
+      </c>
+      <c r="I7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F8">
         <v>1897</v>
       </c>
       <c r="G8">
-        <v>0.85698946993749281</v>
+        <v>0.8569894699374928</v>
       </c>
       <c r="H8">
-        <v>0.90612590208889632</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9061259020888963</v>
+      </c>
+      <c r="I8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F9">
         <v>2101</v>
       </c>
       <c r="G9">
-        <v>0.93373023460337312</v>
+        <v>0.9337302346033731</v>
       </c>
       <c r="H9">
-        <v>0.94768334790136033</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9476833479013603</v>
+      </c>
+      <c r="I9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F10">
         <v>2002</v>
       </c>
       <c r="G10">
-        <v>0.92600776715769129</v>
+        <v>0.9260077671576913</v>
       </c>
       <c r="H10">
-        <v>0.95798433756326962</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9579843375632696</v>
+      </c>
+      <c r="I10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F11">
         <v>1929</v>
       </c>
       <c r="G11">
-        <v>0.87420882386685361</v>
+        <v>0.8742088238668536</v>
       </c>
       <c r="H11">
-        <v>0.77418436510819799</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.774184365108198</v>
+      </c>
+      <c r="I11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F12">
         <v>2081</v>
       </c>
       <c r="G12">
-        <v>0.93748149456626728</v>
+        <v>0.9374814945662673</v>
       </c>
       <c r="H12">
-        <v>0.88206180999602901</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.882061809996029</v>
+      </c>
+      <c r="I12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F13">
         <v>1990</v>
       </c>
       <c r="G13">
-        <v>0.93832846443063844</v>
+        <v>0.9383284644306384</v>
       </c>
       <c r="H13">
-        <v>0.88050442878347279</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.8805044287834728</v>
+      </c>
+      <c r="I13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F14">
         <v>2400</v>
       </c>
       <c r="G14">
-        <v>0.96779374635052429</v>
+        <v>0.9677937463505243</v>
       </c>
       <c r="H14">
-        <v>0.99228986532796737</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9922898653279674</v>
+      </c>
+      <c r="I14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F15">
         <v>2377</v>
       </c>
       <c r="G15">
-        <v>0.96893622338761498</v>
+        <v>0.968936223387615</v>
       </c>
       <c r="H15">
-        <v>0.99344069390505685</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9934406939050568</v>
+      </c>
+      <c r="I15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F16">
         <v>1223</v>
       </c>
       <c r="G16">
-        <v>0.97260395976158265</v>
+        <v>0.9726039597615826</v>
       </c>
       <c r="H16">
-        <v>0.98980258719320324</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9898025871932032</v>
+      </c>
+      <c r="I16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F17">
         <v>2383</v>
       </c>
       <c r="G17">
-        <v>0.97835123372594068</v>
+        <v>0.9783512337259407</v>
       </c>
       <c r="H17">
-        <v>0.90480456234917872</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9048045623491787</v>
+      </c>
+      <c r="I17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F18">
         <v>2417</v>
       </c>
       <c r="G18">
-        <v>0.98572546729446942</v>
+        <v>0.9857254672944694</v>
       </c>
       <c r="H18">
-        <v>0.94560619131728307</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9456061913172831</v>
+      </c>
+      <c r="I18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F19">
         <v>1200</v>
       </c>
       <c r="G19">
-        <v>0.98940524072751135</v>
+        <v>0.9894052407275113</v>
       </c>
       <c r="H19">
         <v>0.9378361317418823</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F20">
         <v>2309</v>
       </c>
       <c r="G20">
-        <v>0.86065168413742243</v>
+        <v>0.8606516841374224</v>
       </c>
       <c r="H20">
-        <v>0.91432855497476262</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9143285549747626</v>
+      </c>
+      <c r="I20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F21">
         <v>2499</v>
       </c>
       <c r="G21">
-        <v>0.89684696253761398</v>
+        <v>0.896846962537614</v>
       </c>
       <c r="H21">
-        <v>0.92698463639110895</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.926984636391109</v>
+      </c>
+      <c r="I21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F22">
         <v>1192</v>
       </c>
       <c r="G22">
-        <v>0.95563275793151914</v>
+        <v>0.9556327579315191</v>
       </c>
       <c r="H22">
-        <v>0.97702172708000934</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9770217270800093</v>
+      </c>
+      <c r="I22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F23">
         <v>2344</v>
       </c>
       <c r="G23">
-        <v>0.87296032613486407</v>
+        <v>0.8729603261348641</v>
       </c>
       <c r="H23">
-        <v>0.77253710748976767</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.7725371074897677</v>
+      </c>
+      <c r="I23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F24">
         <v>2479</v>
       </c>
       <c r="G24">
-        <v>0.90177974120402471</v>
+        <v>0.9017797412040247</v>
       </c>
       <c r="H24">
         <v>0.8327699113557111</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F25">
         <v>1177</v>
       </c>
       <c r="G25">
-        <v>0.94867515969953553</v>
+        <v>0.9486751596995355</v>
       </c>
       <c r="H25">
-        <v>0.88185881643012554</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.8818588164301255</v>
+      </c>
+      <c r="I25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E26" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F26">
         <v>1983</v>
       </c>
       <c r="G26">
-        <v>0.98224009942319079</v>
+        <v>0.9822400994231908</v>
       </c>
       <c r="H26">
-        <v>0.98730680288192929</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9873068028819293</v>
+      </c>
+      <c r="I26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D27" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E27" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F27">
         <v>2014</v>
       </c>
       <c r="G27">
-        <v>0.98752091214862558</v>
+        <v>0.9875209121486256</v>
       </c>
       <c r="H27">
-        <v>0.98484260741884289</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9848426074188429</v>
+      </c>
+      <c r="I27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E28" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F28">
         <v>2003</v>
       </c>
       <c r="G28">
-        <v>0.97080174056763213</v>
+        <v>0.9708017405676321</v>
       </c>
       <c r="H28">
-        <v>0.98934543956289955</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9893454395628996</v>
+      </c>
+      <c r="I28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D29" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F29">
         <v>2008</v>
       </c>
       <c r="G29">
-        <v>0.99279285638671688</v>
+        <v>0.9927928563867169</v>
       </c>
       <c r="H29">
-        <v>0.83146863774836255</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.8314686377483625</v>
+      </c>
+      <c r="I29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D30" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F30">
         <v>1972</v>
       </c>
       <c r="G30">
-        <v>0.98067815415031312</v>
+        <v>0.9806781541503131</v>
       </c>
       <c r="H30">
-        <v>0.91638050593698961</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9163805059369896</v>
+      </c>
+      <c r="I30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C31" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D31" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E31" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F31">
         <v>2020</v>
       </c>
       <c r="G31">
-        <v>0.98719334212441878</v>
+        <v>0.9871933421244188</v>
       </c>
       <c r="H31">
-        <v>0.91093640918622665</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9109364091862266</v>
+      </c>
+      <c r="I31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C32" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D32" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E32" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F32">
         <v>1897</v>
@@ -1339,143 +1412,156 @@
       <c r="H32">
         <v>0.893018296712767</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C33" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D33" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E33" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F33">
         <v>2101</v>
       </c>
       <c r="G33">
-        <v>0.95205490359425282</v>
+        <v>0.9520549035942528</v>
       </c>
       <c r="H33">
-        <v>0.93989310183179486</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9398931018317949</v>
+      </c>
+      <c r="I33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C34" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D34" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E34" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F34">
         <v>2002</v>
       </c>
       <c r="G34">
-        <v>0.92267374941927882</v>
+        <v>0.9226737494192788</v>
       </c>
       <c r="H34">
-        <v>0.95322095979402988</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.9532209597940299</v>
+      </c>
+      <c r="I34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C35" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D35" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E35" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F35">
         <v>1929</v>
       </c>
       <c r="G35">
-        <v>0.87656676354450702</v>
+        <v>0.876566763544507</v>
       </c>
       <c r="H35">
-        <v>0.68640977803820824</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.6864097780382082</v>
+      </c>
+      <c r="I35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C36" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D36" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E36" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F36">
         <v>2081</v>
       </c>
       <c r="G36">
-        <v>0.95190175358801432</v>
+        <v>0.9519017535880143</v>
       </c>
       <c r="H36">
         <v>0.8277898707885657</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C37" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D37" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E37" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F37">
         <v>1990</v>
       </c>
       <c r="G37">
-        <v>0.92583718510977597</v>
+        <v>0.925837185109776</v>
       </c>
       <c r="H37">
-        <v>0.83968554336221779</v>
+        <v>0.8396855433622178</v>
+      </c>
+      <c r="I37" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
-      <formula>0.8</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>